<commit_message>
Das richtige Protokoll 4
</commit_message>
<xml_diff>
--- a/artefacts/protocols/sprint_protocol_4.xlsx
+++ b/artefacts/protocols/sprint_protocol_4.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\studyhelp\protocols\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christian\Documents\xampp3\htdocs\studyhelp\protocols\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{996C05D1-C005-41CD-B7BB-1D5760D429FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30120" windowHeight="12345"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,8 +23,6 @@
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
   <si>
     <t>Sprint Review Protocol</t>
   </si>
@@ -122,16 +119,19 @@
     <t>Richter Georg</t>
   </si>
   <si>
-    <t>Freundesliste um Level der Freunde und Highscores ergänzt</t>
-  </si>
-  <si>
-    <t>die zahl 2.5 wird aus irgendeinem grund in ein datum umgewandelt bei Real Efort [h]</t>
+    <t>Profildaten anzeigen/bearbeiten</t>
+  </si>
+  <si>
+    <t>Vergangene Spielresultate auf dem Profil anzeigen/sortieren</t>
+  </si>
+  <si>
+    <t>Freundesystem erstellen, Freunde hinzufügen etc.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -362,7 +362,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -377,6 +377,33 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -392,12 +419,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -419,28 +440,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -754,11 +753,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -774,28 +773,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
+      <c r="A2" s="19"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
     </row>
     <row r="3" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="5"/>
@@ -809,133 +808,133 @@
       <c r="I3" s="5"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="17">
+      <c r="B4" s="23"/>
+      <c r="C4" s="24">
+        <v>4</v>
+      </c>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="25"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="13"/>
+      <c r="C5" s="26">
+        <v>44698.791666666664</v>
+      </c>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="28"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="13"/>
+      <c r="C6" s="27">
+        <v>21</v>
+      </c>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="28"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="13"/>
+      <c r="C7" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="30"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="13"/>
+      <c r="C8" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="21"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="18"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="16"/>
-      <c r="C5" s="19">
-        <v>44726.791666666664</v>
-      </c>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="21"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="20">
-        <v>21</v>
-      </c>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="21"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="16"/>
-      <c r="C7" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="23"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="16"/>
-      <c r="C8" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="12"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="16"/>
-      <c r="C9" s="11" t="s">
+      <c r="B9" s="13"/>
+      <c r="C9" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="12"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="21"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="11" t="s">
+      <c r="B10" s="13"/>
+      <c r="C10" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="12"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="21"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="16"/>
-      <c r="C11" s="29" t="s">
+      <c r="B11" s="13"/>
+      <c r="C11" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="29"/>
-      <c r="E11" s="29"/>
-      <c r="F11" s="29"/>
-      <c r="G11" s="30"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="18"/>
     </row>
     <row r="12" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="26" t="s">
+      <c r="A12" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="27"/>
-      <c r="C12" s="24" t="s">
+      <c r="B12" s="15"/>
+      <c r="C12" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="24"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="25"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="11"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="28" t="s">
+      <c r="A14" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="28"/>
-      <c r="C14" s="28"/>
-      <c r="D14" s="28"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="28"/>
-      <c r="G14" s="28"/>
-      <c r="H14" s="28"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -971,31 +970,35 @@
         <v>29</v>
       </c>
       <c r="C16" s="7">
-        <v>1</v>
-      </c>
-      <c r="D16" s="31">
-        <v>2.5</v>
+        <v>15</v>
+      </c>
+      <c r="D16" s="7">
+        <v>15</v>
       </c>
       <c r="E16" s="9">
         <f>D16-C16</f>
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="F16" s="3"/>
       <c r="G16" s="4"/>
-      <c r="H16" s="7" t="s">
-        <v>30</v>
-      </c>
+      <c r="H16" s="7"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <v>2</v>
       </c>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
+      <c r="B17" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="7">
+        <v>20</v>
+      </c>
+      <c r="D17" s="7">
+        <v>18</v>
+      </c>
       <c r="E17" s="9">
         <f t="shared" ref="E17:E25" si="0">D17-C17</f>
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="4"/>
@@ -1005,12 +1008,18 @@
       <c r="A18" s="8">
         <v>3</v>
       </c>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
+      <c r="B18" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" s="7">
+        <v>25</v>
+      </c>
+      <c r="D18" s="7">
+        <v>24</v>
+      </c>
       <c r="E18" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F18" s="3"/>
       <c r="G18" s="4"/>
@@ -1131,7 +1140,7 @@
       <c r="D26" s="6"/>
       <c r="E26" s="6">
         <f>SUM(E16:E25)</f>
-        <v>1.5</v>
+        <v>-3</v>
       </c>
       <c r="F26" s="6">
         <f>COUNT(F16:F25)</f>
@@ -1156,12 +1165,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A14:H14"/>
-    <mergeCell ref="C11:G11"/>
     <mergeCell ref="A1:I2"/>
     <mergeCell ref="C9:G9"/>
     <mergeCell ref="C10:G10"/>
@@ -1176,6 +1179,12 @@
     <mergeCell ref="C6:G6"/>
     <mergeCell ref="C7:G7"/>
     <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A14:H14"/>
+    <mergeCell ref="C11:G11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>